<commit_message>
lib + read file excel
đọc file excel để thay đổi lượng tiêu dùng trong các dịch vụ
</commit_message>
<xml_diff>
--- a/Hoa_don_tien_dien.xlsx
+++ b/Hoa_don_tien_dien.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thanh\Downloads\SP2025\SWP391\apartment-management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CED57D3-BBB9-49A8-85CC-A7DF4DC8AC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB9D818F-7F60-4744-A17C-54F36DAAC66D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2FE0AE2C-218A-484F-9B00-587A51F1B144}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t>Apartment</t>
   </si>
@@ -43,16 +43,60 @@
   </si>
   <si>
     <t xml:space="preserve">Đơn vị </t>
+  </si>
+  <si>
+    <t>A01_01</t>
+  </si>
+  <si>
+    <t>A09_01</t>
+  </si>
+  <si>
+    <t>A10_04</t>
+  </si>
+  <si>
+    <t>A10_01</t>
+  </si>
+  <si>
+    <t>A11_02</t>
+  </si>
+  <si>
+    <t>A11_03</t>
+  </si>
+  <si>
+    <t>A09_04</t>
+  </si>
+  <si>
+    <t>A09_03</t>
+  </si>
+  <si>
+    <t>A10_06</t>
+  </si>
+  <si>
+    <t>kWh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -75,13 +119,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -394,29 +446,130 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83CD89E6-1579-4383-A295-60844341CF19}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="23.88671875" customWidth="1"/>
+    <col min="1" max="2" width="23.88671875" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>100</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>100</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>100</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>100</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1">
+        <v>100</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1">
+        <v>100</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1">
+        <v>100</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1">
+        <v>100</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1">
+        <v>100</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update login invoice generate
</commit_message>
<xml_diff>
--- a/Hoa_don_tien_dien.xlsx
+++ b/Hoa_don_tien_dien.xlsx
@@ -38,22 +38,22 @@
     <t xml:space="preserve">Đơn vị </t>
   </si>
   <si>
+    <t>A11_02</t>
+  </si>
+  <si>
+    <t>kWh</t>
+  </si>
+  <si>
+    <t>A01_01</t>
+  </si>
+  <si>
     <t>A10_04</t>
   </si>
   <si>
-    <t>kWh</t>
-  </si>
-  <si>
-    <t>A01_01</t>
-  </si>
-  <si>
     <t>A09_01</t>
   </si>
   <si>
     <t>A10_01</t>
-  </si>
-  <si>
-    <t>A11_02</t>
   </si>
   <si>
     <t>A11_03</t>
@@ -73,10 +73,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -543,16 +543,16 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1013,7 +1013,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="2"/>
@@ -1038,7 +1038,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1">
-        <v>23542</v>
+        <v>500</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
@@ -1049,7 +1049,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="1">
-        <v>3435</v>
+        <v>344</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
@@ -1060,7 +1060,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>3333</v>
+        <v>123</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
@@ -1071,7 +1071,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="1">
-        <v>100</v>
+        <v>542</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
@@ -1082,7 +1082,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="1">
-        <v>100</v>
+        <v>123</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
@@ -1093,7 +1093,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="1">
-        <v>100</v>
+        <v>455</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
@@ -1104,7 +1104,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="1">
-        <v>100</v>
+        <v>234</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>4</v>
@@ -1115,7 +1115,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="1">
-        <v>100</v>
+        <v>543</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>4</v>
@@ -1126,7 +1126,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="1">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
update get service id (dien+nuoc)
</commit_message>
<xml_diff>
--- a/Hoa_don_tien_dien.xlsx
+++ b/Hoa_don_tien_dien.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
   <si>
     <t>Apartment</t>
   </si>
@@ -38,34 +38,67 @@
     <t xml:space="preserve">Đơn vị </t>
   </si>
   <si>
-    <t>A11_02</t>
+    <t>A001</t>
   </si>
   <si>
     <t>kWh</t>
   </si>
   <si>
-    <t>A01_01</t>
-  </si>
-  <si>
-    <t>A10_04</t>
-  </si>
-  <si>
-    <t>A09_01</t>
-  </si>
-  <si>
-    <t>A10_01</t>
-  </si>
-  <si>
-    <t>A11_03</t>
-  </si>
-  <si>
-    <t>A09_04</t>
-  </si>
-  <si>
-    <t>A09_03</t>
-  </si>
-  <si>
-    <t>A10_06</t>
+    <t>A002</t>
+  </si>
+  <si>
+    <t>A003</t>
+  </si>
+  <si>
+    <t>A004</t>
+  </si>
+  <si>
+    <t>A005</t>
+  </si>
+  <si>
+    <t>A006</t>
+  </si>
+  <si>
+    <t>A007</t>
+  </si>
+  <si>
+    <t>A008</t>
+  </si>
+  <si>
+    <t>A009</t>
+  </si>
+  <si>
+    <t>A010</t>
+  </si>
+  <si>
+    <t>A011</t>
+  </si>
+  <si>
+    <t>A012</t>
+  </si>
+  <si>
+    <t>A013</t>
+  </si>
+  <si>
+    <t>A014</t>
+  </si>
+  <si>
+    <t>A015</t>
+  </si>
+  <si>
+    <t>A016</t>
+  </si>
+  <si>
+    <t>A017</t>
+  </si>
+  <si>
+    <t>A018</t>
+  </si>
+  <si>
+    <t>A019</t>
+  </si>
+  <si>
+    <t>A020</t>
   </si>
 </sst>
 </file>
@@ -1010,10 +1043,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A10"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="2"/>
@@ -1056,7 +1089,7 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1">
@@ -1067,7 +1100,7 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1">
@@ -1078,7 +1111,7 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1">
@@ -1089,7 +1122,7 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="1">
@@ -1100,7 +1133,7 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="1">
@@ -1111,7 +1144,7 @@
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="1">
@@ -1122,7 +1155,7 @@
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="1">
@@ -1131,6 +1164,130 @@
       <c r="C10" s="1" t="s">
         <v>4</v>
       </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1">
+        <v>500</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1">
+        <v>344</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1">
+        <v>123</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1">
+        <v>542</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1">
+        <v>123</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="1">
+        <v>455</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="1">
+        <v>234</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="1">
+        <v>543</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="1">
+        <v>121</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="1">
+        <v>543</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="1">
+        <v>121</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>